<commit_message>
models_summary for PnL and VIX
</commit_message>
<xml_diff>
--- a/reports/calibrations/models_summary_PnL-VIX-LogDiff.xlsx
+++ b/reports/calibrations/models_summary_PnL-VIX-LogDiff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Documents\git\dynamic-trading\reports\calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AB11E0-5ADC-4718-94C4-9FB6C7B529DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC13F97D-6085-455F-87A0-534A9180F6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pivot" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -199,12 +199,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -234,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -247,22 +253,23 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2640,157 +2647,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48FFBAE4-564D-4B15-BF7A-9FCB17B64BA7}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A4:C19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="16">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="15">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="8"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="8">
-        <item x="2"/>
-        <item x="6"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="14">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of rsquared" fld="14" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="0">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <conditionalFormats count="1">
-    <conditionalFormat priority="3">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-  </conditionalFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{343934BB-4111-4521-BE39-294706D15A18}" name="PivotTable2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{343934BB-4111-4521-BE39-294706D15A18}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D5:F19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="16">
     <pivotField axis="axisRow" showAll="0">
@@ -2912,10 +2769,10 @@
     <dataField name="Sum of nobs" fld="6" baseField="0" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="1">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2924,7 +2781,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2934,6 +2791,156 @@
       </pivotArea>
     </format>
   </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48FFBAE4-564D-4B15-BF7A-9FCB17B64BA7}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A4:C19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="16">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="8">
+        <item x="2"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="14">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of rsquared" fld="14" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="3">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <conditionalFormats count="1">
+    <conditionalFormat priority="3">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -3269,8 +3276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822FB108-9E72-4F02-A4B1-0052FAC1E48D}">
   <dimension ref="A2:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H13" activeCellId="1" sqref="H15 H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3429,7 +3436,7 @@
         <f t="shared" si="0"/>
         <v>-0.76113850038992759</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="8" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3528,7 +3535,7 @@
         <f t="shared" si="0"/>
         <v>-6.8488116156690824</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="8" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3555,7 +3562,7 @@
         <f t="shared" si="0"/>
         <v>-3.7448339172142711</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="8" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3582,7 +3589,7 @@
         <f t="shared" si="0"/>
         <v>-3.5025525991342623</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="8" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3609,7 +3616,7 @@
         <f t="shared" si="0"/>
         <v>1.6094431907192408</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="8" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3636,7 +3643,7 @@
         <f t="shared" si="0"/>
         <v>-1.8217347818440712</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="8" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3687,7 +3694,7 @@
         <f t="shared" si="0"/>
         <v>-4.9876375586873571</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="8" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>